<commit_message>
import cases within web
</commit_message>
<xml_diff>
--- a/TestCase/Sample Excel Test Sheet.xlsx
+++ b/TestCase/Sample Excel Test Sheet.xlsx
@@ -85,7 +85,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -98,13 +98,9 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="9"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -130,14 +126,11 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -528,7 +521,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -591,7 +586,6 @@
       <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -603,7 +597,6 @@
       <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -629,7 +622,6 @@
       <c r="D6" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -641,7 +633,6 @@
       <c r="D7" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -667,7 +658,6 @@
       <c r="D9" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -679,11 +669,10 @@
       <c r="D10" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="2"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>